<commit_message>
update laserCutBox & add spirals.py
1. added spirals.py program to the repo
2. modified laserCutBox.py to include smaller functions
3. added functions for user text (top, front)
</commit_message>
<xml_diff>
--- a/laserCutBoxCases.xlsx
+++ b/laserCutBoxCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yehuda/GitHub/laser_cutting/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7A287EA-5CEA-BA48-8E74-BBE7D502D035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD65B94-1A85-A94D-8B73-7928E7B7E4C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14400" xr2:uid="{EE1D6688-7C64-A140-8986-C66AAEC9673E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="19">
   <si>
     <t>W</t>
   </si>
@@ -73,6 +73,24 @@
   </si>
   <si>
     <t>Shortest</t>
+  </si>
+  <si>
+    <t>W x L</t>
+  </si>
+  <si>
+    <t>W x H</t>
+  </si>
+  <si>
+    <t>H x L</t>
+  </si>
+  <si>
+    <t>Pieces</t>
+  </si>
+  <si>
+    <t>Assumes:</t>
+  </si>
+  <si>
+    <t>Partition is width-wise (front compartment, back compartment)</t>
   </si>
 </sst>
 </file>
@@ -152,6 +170,512 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>433320</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>15175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>671575</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>73720</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:am3d="http://schemas.microsoft.com/office/drawing/2017/model3d" Requires="am3d">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="3D Model 1" descr="Red Cuboid">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEE06879-5C44-7C4C-A9B3-177ECFE39EBA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr>
+              <a:graphicFrameLocks noChangeAspect="1"/>
+            </xdr:cNvGraphicFramePr>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2017/model3d">
+              <am3d:model3d xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+                <am3d:spPr>
+                  <a:xfrm>
+                    <a:off x="0" y="0"/>
+                    <a:ext cx="2714755" cy="2496945"/>
+                  </a:xfrm>
+                  <a:prstGeom prst="rect">
+                    <a:avLst/>
+                  </a:prstGeom>
+                </am3d:spPr>
+                <am3d:camera>
+                  <am3d:pos x="0" y="0" z="57664451"/>
+                  <am3d:up dx="0" dy="36000000" dz="0"/>
+                  <am3d:lookAt x="0" y="0" z="0"/>
+                  <am3d:perspective fov="2700000"/>
+                </am3d:camera>
+                <am3d:trans>
+                  <am3d:meterPerModelUnit n="4361393" d="1000000"/>
+                  <am3d:preTrans dx="0" dy="-6493603" dz="0"/>
+                  <am3d:scale>
+                    <am3d:sx n="1000000" d="1000000"/>
+                    <am3d:sy n="1000000" d="1000000"/>
+                    <am3d:sz n="1000000" d="1000000"/>
+                  </am3d:scale>
+                  <am3d:rot ax="8700000" ay="1800000" az="9600000"/>
+                  <am3d:postTrans dx="0" dy="0" dz="0"/>
+                </am3d:trans>
+                <am3d:raster rName="Office3DRenderer" rVer="16.0.8326">
+                  <am3d:blip r:embed="rId2"/>
+                </am3d:raster>
+                <am3d:objViewport viewportSz="2743195"/>
+                <am3d:ambientLight>
+                  <am3d:clr>
+                    <a:scrgbClr r="50000" g="50000" b="50000"/>
+                  </am3d:clr>
+                  <am3d:illuminance n="500000" d="1000000"/>
+                </am3d:ambientLight>
+                <am3d:ptLight rad="0">
+                  <am3d:clr>
+                    <a:scrgbClr r="100000" g="75000" b="50000"/>
+                  </am3d:clr>
+                  <am3d:intensity n="9765625" d="1000000"/>
+                  <am3d:pos x="21959998" y="70920001" z="16344003"/>
+                </am3d:ptLight>
+                <am3d:ptLight rad="0">
+                  <am3d:clr>
+                    <a:scrgbClr r="40000" g="60000" b="95000"/>
+                  </am3d:clr>
+                  <am3d:intensity n="12250000" d="1000000"/>
+                  <am3d:pos x="-37964106" y="51130435" z="57631972"/>
+                </am3d:ptLight>
+                <am3d:ptLight rad="0">
+                  <am3d:clr>
+                    <a:scrgbClr r="86837" g="72700" b="100000"/>
+                  </am3d:clr>
+                  <am3d:intensity n="3125000" d="1000000"/>
+                  <am3d:pos x="-37739122" y="58056624" z="-34769649"/>
+                </am3d:ptLight>
+              </am3d:model3d>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="3D Model 1" descr="Red Cuboid">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEE06879-5C44-7C4C-A9B3-177ECFE39EBA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr>
+              <a:picLocks noGrp="1" noRot="1" noChangeAspect="1" noMove="1" noResize="1" noEditPoints="1" noAdjustHandles="1" noChangeArrowheads="1" noChangeShapeType="1" noCrop="1"/>
+            </xdr:cNvPicPr>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7862820" y="2250375"/>
+              <a:ext cx="2714755" cy="2496945"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>520</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>46880</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>363400</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>14160</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="5" name="Ink 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E129C972-3CA0-F04B-98BA-4DE9B0D5870F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="8255520" y="4517280"/>
+            <a:ext cx="362880" cy="373680"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="5" name="Ink 4">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E129C972-3CA0-F04B-98BA-4DE9B0D5870F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="8246880" y="4508640"/>
+              <a:ext cx="380520" cy="391320"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>235980</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>116800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>391500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>94880</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="10" name="Ink 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0FE67E6-C1D4-6D4A-A00C-FD0514FF0947}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7665480" y="3571200"/>
+            <a:ext cx="155520" cy="384480"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="10" name="Ink 9">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0FE67E6-C1D4-6D4A-A00C-FD0514FF0947}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7656840" y="3562560"/>
+              <a:ext cx="173160" cy="402120"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>720860</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>80680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>141240</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>72440</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="11" name="Ink 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{610A537C-109A-4343-8302-24A5653638CA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="9801360" y="4144680"/>
+            <a:ext cx="245880" cy="398160"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="11" name="Ink 10">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{610A537C-109A-4343-8302-24A5653638CA}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="9792720" y="4136040"/>
+              <a:ext cx="263520" cy="415800"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>270760</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>130800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>271120</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>131160</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="24" name="Ink 23">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F491654-2BC3-7A4C-8F59-DDC8EE6BBF89}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="13478760" y="3178800"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="24" name="Ink 23">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F491654-2BC3-7A4C-8F59-DDC8EE6BBF89}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13469760" y="3170160"/>
+              <a:ext cx="18000" cy="18000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-02-06T19:06:18.415"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'0'22'0,"3"17"0,6 23 0,10 14 0,8 2 0,4-3 0,-2-8 0,0-4 0,-1-1 0,0 2 0,0 0 0,-3-4 0,-2-11 0,-6-11 0,-6-9 0,-4-8 0,-3-4 0,-2-5 0,2-5 0,1-4 0,2-1 0,4-4 0,3-7 0,3-8 0,2-11 0,2-8 0,-3 0 0,-2 2 0,-4 6 0,-1 6 0,-6 7 0,-1 5 0,-4 4 0,2-4 0,2-3 0,1-4 0,2-1 0,-3-1 0,0 1 0,-1-1 0,0 3 0,-1 4 0,2 5 0,-1 8 0,2 17 0,3 18 0,3 26 0,3 13 0,2 3 0,0-9 0,-2-19 0,0-12 0,0-14 0,-1-4 0,-1-3 0,-1-3 0,-3-5 0,-2-4 0,-1-3 0,0-1 0,3-1 0,4 0 0,4-4 0,7-19 0,4-22 0,8-37 0,-14 28 0,-1-2 0,1-2 0,-1 1 0,0 2 0,-2 3 0,10-27 0,-8 27 0,-8 23 0,-6 13 0,-4 8 0,-1 6 0,-1 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-02-06T19:06:20.717"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'0'22'0,"0"8"0,0 12 0,0 9 0,0 3 0,0 3 0,2-2 0,3-3 0,1-6 0,-1-8 0,-3-4 0,-1-5 0,-1 0 0,0-3 0,0-3 0,0-2 0,0-3 0,0-4 0,0-3 0,0-2 0,0 2 0,0 3 0,0 6 0,0 4 0,0 3 0,2 1 0,0-4 0,1-3 0,-1-3 0,-2 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0-4 0,0-2 0,0-7 0,0-2 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1449">31 546 24575,'8'0'0,"1"0"0,-1 0 0,3 0 0,1 0 0,-1 0 0,0 0 0,-1 0 0,2 0 0,3 0 0,2 0 0,1 0 0,2 0 0,-2 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,-2 0 0,-2 0 0,-1 0 0,-2 0 0,-2 0 0,-2 0-6784,-2 0 6784,0 0 0,-3 0 0,0 0 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3201">414 153 24575,'0'30'0,"0"1"0,0 3 0,0 2 0,0 8 0,0 3 0,0 2 0,0 2 0,0-3 0,0-8 0,0-8 0,0 1 0,0 3 0,0 0 0,0 1 0,0-9 0,0-3 0,0 1 0,0 0 0,2-2 0,0 2 0,1 0 0,-1 0 0,-2 0 0,2-1 0,0-3 0,1-3 0,-1-6 0,-2-4 0,0-4 0,0-3 0,0 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-02-06T19:06:27.053"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 1 24575,'0'16'0,"2"12"0,4 13 0,9 36 0,-5-37 0,6 37 0,-11-33 0,0 17 0,-1 6 0,-1-11 0,0 0 0,2 0 0,-1 1 0,-1-4 0,-1-1 0,-2-2 0,0-7 0,0-1 0,0-7 0,0-5 0,0-3 0,0-4 0,0-3 0,0 4 0,0-10 0,0 0 0,3-12 0,12-8 0,16-11 0,14-6 0,6-4 0,-1 4 0,-3 3 0,-3 2 0,0 3 0,-4 4 0,-2 3 0,-4 5 0,-4 0 0,-1 3 0,-3 0 0,-2 0 0,-2 0 0,-11 0 0,0 0 0,-9 0 0,0 0 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2022-02-06T19:08:02.410"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 1 24575,'0'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4E6408FD-E8B6-1E4E-ACF1-27328BACBEF7}" name="Table1" displayName="Table1" ref="B3:G27" totalsRowShown="0" dataDxfId="0">
   <autoFilter ref="B3:G27" xr:uid="{4E6408FD-E8B6-1E4E-ACF1-27328BACBEF7}"/>
@@ -162,6 +686,24 @@
     <tableColumn id="4" xr3:uid="{A0363942-2EE8-324A-8451-5E1D9511CC77}" name="Shortest" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{5AC00C4A-C920-AA43-AD34-981FB026A238}" name="Lid" dataDxfId="2"/>
     <tableColumn id="6" xr3:uid="{E993CF15-1ECA-9245-9EF9-19CEF6704418}" name="Partition" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{543E8B25-AF6D-0247-9C06-908C8AB58E49}" name="Table2" displayName="Table2" ref="J3:P7" totalsRowShown="0">
+  <autoFilter ref="J3:P7" xr:uid="{543E8B25-AF6D-0247-9C06-908C8AB58E49}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{860F9562-81E0-A649-AF94-5DB98A14385E}" name="Case"/>
+    <tableColumn id="2" xr3:uid="{034D9883-B8FF-8147-A5E5-2DD4D6709B5A}" name="Lid"/>
+    <tableColumn id="3" xr3:uid="{25C2BCAD-427F-F44C-A1B2-8D70DE773833}" name="Partition"/>
+    <tableColumn id="4" xr3:uid="{56AA6F38-8ABA-9147-88B1-69CC7E795842}" name="W x L"/>
+    <tableColumn id="5" xr3:uid="{1CC04CF7-734A-4248-A25C-9D0E7D7F048D}" name="W x H"/>
+    <tableColumn id="6" xr3:uid="{EBB5CDE3-972F-D148-A6DB-D85E41636095}" name="H x L"/>
+    <tableColumn id="7" xr3:uid="{F16BC0A6-7A40-D843-BF49-41D21119F50C}" name="Pieces">
+      <calculatedColumnFormula>SUM(M4:O4)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -464,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FA53318-880B-864F-99BC-F622EED7EA2A}">
-  <dimension ref="B3:G27"/>
+  <dimension ref="B3:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -479,7 +1021,7 @@
     <col min="7" max="7" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>9</v>
       </c>
@@ -498,8 +1040,29 @@
       <c r="G3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M3" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" t="s">
+        <v>14</v>
+      </c>
+      <c r="O3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -518,8 +1081,30 @@
       <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>2</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <f>SUM(M4:O4)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -538,8 +1123,30 @@
       <c r="G5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>2</v>
+      </c>
+      <c r="K5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>3</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5">
+        <f>SUM(M5:O5)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -558,8 +1165,30 @@
       <c r="G6" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6">
+        <v>2</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+      <c r="O6">
+        <v>2</v>
+      </c>
+      <c r="P6">
+        <f>SUM(M6:O6)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -578,8 +1207,30 @@
       <c r="G7" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" t="s">
+        <v>6</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <v>3</v>
+      </c>
+      <c r="O7">
+        <v>2</v>
+      </c>
+      <c r="P7">
+        <f>SUM(M7:O7)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -599,7 +1250,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -618,8 +1269,11 @@
       <c r="G9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>7</v>
       </c>
@@ -638,8 +1292,14 @@
       <c r="G10" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>8</v>
       </c>
@@ -659,7 +1319,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>9</v>
       </c>
@@ -679,7 +1339,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>10</v>
       </c>
@@ -699,7 +1359,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B14" s="1">
         <v>11</v>
       </c>
@@ -719,7 +1379,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
         <v>12</v>
       </c>
@@ -739,7 +1399,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
         <v>13</v>
       </c>
@@ -981,8 +1641,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>